<commit_message>
fix tinyint,dateformat. start customData.
</commit_message>
<xml_diff>
--- a/QueryReport/excelTemplate/Employee_-__Listwhy_20200224120000_(1)_20200224120000.xlsx
+++ b/QueryReport/excelTemplate/Employee_-__Listwhy_20200224120000_(1)_20200224120000.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C1E427-03FB-4DAA-AD08-B92C98339F07}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Report" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="0"/>
-</workbook>
+  <x:bookViews>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Report" sheetId="1" r:id="rId1"/>
+  </x:sheets>
+  <x:calcPr calcId="0"/>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -121,87 +121,108 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
-  <fonts count="4">
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Microsoft YaHei"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Microsoft YaHei"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Microsoft YaHei"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-  </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="177" formatCode="yyyy\-mm\-dd;@"/>
+    <x:numFmt numFmtId="240" formatCode="yyyy-mm-dd"/>
+  </x:numFmts>
+  <x:fonts count="6">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Microsoft YaHei"/>
+    </x:font>
+    <x:font>
+      <x:sz val="9"/>
+      <x:name val="宋体"/>
+      <x:family val="3"/>
+      <x:charset val="134"/>
+    </x:font>
+    <x:font>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Microsoft YaHei"/>
+      <x:family val="2"/>
+      <x:charset val="134"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Microsoft YaHei"/>
+      <x:family val="2"/>
+      <x:charset val="134"/>
+    </x:font>
+    <x:font>
+      <x:name val="Microsoft YaHei"/>
+      <x:sz val="11"/>
+      <x:color rgb="000000"/>
+    </x:font>
+    <x:font>
+      <x:name val="Microsoft YaHei"/>
+      <x:sz val="11"/>
+      <x:b/>
+      <x:color rgb="000000"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="3">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFFFFF"/>
+      </x:patternFill>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="11">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <x:xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <x:xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <x:xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <x:xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf fontId="4" borderId="0" applyFont="1"/>
+    <x:xf fontId="4" fillId="2" borderId="0" applyFont="1" applyFill="1"/>
+    <x:xf fontId="5" borderId="0" applyFont="1"/>
+    <x:xf numFmtId="240" fontId="4" borderId="0" applyNumberFormat="1" applyFont="1"/>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:dxfs count="0"/>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -500,137 +521,139 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:S2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <cols>
-    <col min="6" max="6" width="24.6640625" style="6" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="5">
-        <v>43661</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0.61639999999999995</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="1">
-        <v>12000</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="3">
-        <v>43661</v>
-      </c>
-      <c r="O2" s="3">
-        <v>52963</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr codeName="Sheet1"/>
+  <x:dimension ref="A1:S2"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="F1" sqref="F1:F1048576"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="16.5"/>
+  <x:cols>
+    <x:col min="6" max="6" width="24.6640625" style="6" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1">
+      <x:c s="9" t="str">
+        <x:v>Contract Description</x:v>
+      </x:c>
+      <x:c s="9" t="str">
+        <x:v>Staff Number</x:v>
+      </x:c>
+      <x:c s="9" t="str">
+        <x:v>English Name</x:v>
+      </x:c>
+      <x:c s="9" t="str">
+        <x:v>Zone Name</x:v>
+      </x:c>
+      <x:c s="9" t="str">
+        <x:v>Position Name</x:v>
+      </x:c>
+      <x:c s="9" t="str">
+        <x:v>Join Date</x:v>
+      </x:c>
+      <x:c s="9" t="str">
+        <x:v>Year of Service</x:v>
+      </x:c>
+      <x:c s="9" t="str">
+        <x:v>Annual Leave Class</x:v>
+      </x:c>
+      <x:c s="9" t="str">
+        <x:v>Holiday Type</x:v>
+      </x:c>
+      <x:c s="9" t="str">
+        <x:v>Employment Type</x:v>
+      </x:c>
+      <x:c s="9" t="str">
+        <x:v>Basic Salary</x:v>
+      </x:c>
+      <x:c s="9" t="str">
+        <x:v>Pay Scale Point</x:v>
+      </x:c>
+      <x:c s="9" t="str">
+        <x:v>PayScale Scheme</x:v>
+      </x:c>
+      <x:c s="9" t="str">
+        <x:v>Commence Date</x:v>
+      </x:c>
+      <x:c s="9" t="str">
+        <x:v>Terminate Date</x:v>
+      </x:c>
+      <x:c s="9" t="str">
+        <x:v>Staff Status</x:v>
+      </x:c>
+      <x:c s="9" t="str">
+        <x:v>Part Time</x:v>
+      </x:c>
+      <x:c s="9" t="str">
+        <x:v>SecurityGroupID</x:v>
+      </x:c>
+      <x:c s="9" t="str">
+        <x:v>Securtiy Group</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2">
+      <x:c s="7" t="str">
+        <x:v>Data World Solutions Ltd</x:v>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v>AA100002</x:v>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v>Test One</x:v>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v>Unit A</x:v>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v>保健員</x:v>
+      </x:c>
+      <x:c s="10" t="d">
+        <x:v>2019-07-15T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c s="7" t="n">
+        <x:v>0.6164</x:v>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v>AL07</x:v>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v>Bank Holiday</x:v>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v>Monthly</x:v>
+      </x:c>
+      <x:c s="7" t="n">
+        <x:v>12000</x:v>
+      </x:c>
+      <x:c s="7" t="n">
+        <x:v/>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v/>
+      </x:c>
+      <x:c s="10" t="d">
+        <x:v>2019-07-15T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c s="10" t="d">
+        <x:v>2045-01-01T00:00:00.0000000</x:v>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v>Active</x:v>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v>No</x:v>
+      </x:c>
+      <x:c s="7" t="n">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v>DWS - CWB</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:phoneticPr fontId="1" type="noConversion"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</x:worksheet>
 </file>
</xml_diff>